<commit_message>
Refactored document checker (class to instance methods) and added hyperlink checking
</commit_message>
<xml_diff>
--- a/test_results/documentpropertychecker_output.xlsx
+++ b/test_results/documentpropertychecker_output.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -240,15 +240,9 @@
     <t>[Character Reference, Contact Number, Juana Ramirez, 0911-111-2222]</t>
   </si>
   <si>
-    <t>Property HYPERLINK does not exist!</t>
-  </si>
-  <si>
     <t>Personal Website</t>
   </si>
   <si>
-    <t>HYPERLINK=</t>
-  </si>
-  <si>
     <t>Property BORDER BOTTOM does not exist!</t>
   </si>
   <si>
@@ -286,6 +280,9 @@
   </si>
   <si>
     <t>QUESTION 14</t>
+  </si>
+  <si>
+    <t>HYPERLINK=http://www.teachmartin.tk/</t>
   </si>
 </sst>
 </file>
@@ -2034,9 +2031,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2115,32 +2114,35 @@
       <c r="A10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" t="b">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>31</v>
+      </c>
+      <c r="B14" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -2148,7 +2150,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -2156,7 +2158,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -2164,7 +2166,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
@@ -2172,334 +2174,334 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" t="b">
-        <v>1</v>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23">
+      <c r="A22">
         <v>1035063468</v>
       </c>
-      <c r="B23" t="b">
-        <v>1</v>
+      <c r="B22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" t="b">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" t="b">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
         <v>37</v>
       </c>
-      <c r="B31" t="b">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="B30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
         <v>9</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" t="s">
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
         <v>38</v>
       </c>
-      <c r="B33" t="b">
-        <v>1</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="B32" t="b">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
         <v>9</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" t="s">
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
         <v>39</v>
       </c>
-      <c r="B35" t="b">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="B34" t="b">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
         <v>9</v>
       </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" t="s">
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
         <v>40</v>
       </c>
-      <c r="B37" t="b">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="B36" t="b">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
         <v>9</v>
       </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" t="s">
         <v>48</v>
       </c>
-      <c r="B41" t="b">
-        <v>1</v>
+      <c r="B40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" t="b">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" t="b">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>79</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" t="b">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" t="b">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" t="b">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44" t="b">
-        <v>1</v>
-      </c>
-      <c r="C44" t="s">
-        <v>16</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" t="s">
-        <v>51</v>
-      </c>
-      <c r="B46" t="b">
-        <v>1</v>
-      </c>
-      <c r="C46" t="s">
-        <v>81</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" t="s">
-        <v>52</v>
-      </c>
-      <c r="B48" t="b">
-        <v>1</v>
-      </c>
-      <c r="C48" t="s">
-        <v>16</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="E48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" t="s">
-        <v>53</v>
-      </c>
-      <c r="B50" t="b">
-        <v>1</v>
-      </c>
-      <c r="C50" t="s">
-        <v>16</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="E50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" t="s">
-        <v>54</v>
-      </c>
-      <c r="B52" t="b">
-        <v>1</v>
-      </c>
-      <c r="C52" t="s">
-        <v>16</v>
-      </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-      <c r="E52">
-        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" t="s">
         <v>42</v>
       </c>
-      <c r="B56" t="b">
-        <v>1</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="B55" t="b">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
         <v>12</v>
       </c>
-      <c r="D56">
-        <v>1</v>
-      </c>
-      <c r="E56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" t="s">
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
         <v>43</v>
       </c>
-      <c r="B58" t="b">
-        <v>1</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="B57" t="b">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
         <v>12</v>
       </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
-      <c r="E58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" t="s">
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
         <v>44</v>
       </c>
-      <c r="B60" t="b">
-        <v>1</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="B59" t="b">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
         <v>12</v>
       </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" t="s">
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
         <v>45</v>
       </c>
-      <c r="B62" t="b">
-        <v>1</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="B61" t="b">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
         <v>12</v>
       </c>
-      <c r="D62">
-        <v>1</v>
-      </c>
-      <c r="E62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" t="s">
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
         <v>46</v>
       </c>
-      <c r="B64" t="b">
-        <v>1</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="B63" t="b">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
         <v>12</v>
       </c>
-      <c r="D64">
-        <v>1</v>
-      </c>
-      <c r="E64">
-        <v>1</v>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="B67" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B68" t="b">
         <v>1</v>
@@ -2507,7 +2509,7 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B69" t="b">
         <v>1</v>
@@ -2515,34 +2517,37 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
+        <v>85</v>
+      </c>
+      <c r="B70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
         <v>86</v>
-      </c>
-      <c r="B70" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" t="s">
-        <v>87</v>
-      </c>
-      <c r="B71" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>88</v>
+        <v>18</v>
+      </c>
+      <c r="B73" t="b">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s">
+        <v>20</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" t="s">
-        <v>18</v>
-      </c>
-      <c r="B74" t="b">
-        <v>1</v>
-      </c>
       <c r="C74" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -2553,7 +2558,7 @@
     </row>
     <row r="75" spans="1:5">
       <c r="C75" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -2564,23 +2569,12 @@
     </row>
     <row r="76" spans="1:5">
       <c r="C76" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D76">
         <v>1</v>
       </c>
       <c r="E76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="C77" t="s">
-        <v>23</v>
-      </c>
-      <c r="D77">
-        <v>1</v>
-      </c>
-      <c r="E77">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added checking for border bottom
</commit_message>
<xml_diff>
--- a/test_results/documentpropertychecker_output.xlsx
+++ b/test_results/documentpropertychecker_output.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="86">
   <si>
     <t>Name</t>
   </si>
@@ -241,12 +241,6 @@
   </si>
   <si>
     <t>Personal Website</t>
-  </si>
-  <si>
-    <t>Property BORDER BOTTOM does not exist!</t>
-  </si>
-  <si>
-    <t>BORDER BOTTOM=</t>
   </si>
   <si>
     <t>QUESTION 9</t>
@@ -1496,8 +1490,543 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="b">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="b">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="b">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="b">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" t="b">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" t="b">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" t="b">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" t="b">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" t="b">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" t="b">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" t="b">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" t="b">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" t="b">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60" t="b">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s">
+        <v>61</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="C61" t="s">
+        <v>62</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="C62" t="s">
+        <v>63</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="C63" t="s">
+        <v>64</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>59</v>
+      </c>
+      <c r="B67" t="b">
+        <v>1</v>
+      </c>
+      <c r="C67" t="s">
+        <v>25</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1525,7 +2054,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1535,543 +2064,6 @@
       <c r="B3" t="b">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="C7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="C10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="b">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="C13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" t="b">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="C16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" t="b">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" t="b">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" t="b">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" t="b">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" t="b">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" t="b">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" t="b">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" t="s">
-        <v>45</v>
-      </c>
-      <c r="B36" t="b">
-        <v>1</v>
-      </c>
-      <c r="C36" t="s">
-        <v>12</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38" t="b">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" t="s">
-        <v>48</v>
-      </c>
-      <c r="B42" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" t="b">
-        <v>1</v>
-      </c>
-      <c r="C45" t="s">
-        <v>16</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="E45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47" t="b">
-        <v>1</v>
-      </c>
-      <c r="C47" t="s">
-        <v>16</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" t="b">
-        <v>1</v>
-      </c>
-      <c r="C49" t="s">
-        <v>16</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" t="s">
-        <v>53</v>
-      </c>
-      <c r="B51" t="b">
-        <v>1</v>
-      </c>
-      <c r="C51" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-      <c r="E51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" t="s">
-        <v>54</v>
-      </c>
-      <c r="B53" t="b">
-        <v>1</v>
-      </c>
-      <c r="C53" t="s">
-        <v>16</v>
-      </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-      <c r="E53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" t="s">
-        <v>56</v>
-      </c>
-      <c r="B57" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" t="s">
-        <v>18</v>
-      </c>
-      <c r="B60" t="b">
-        <v>1</v>
-      </c>
-      <c r="C60" t="s">
-        <v>61</v>
-      </c>
-      <c r="D60">
-        <v>0</v>
-      </c>
-      <c r="E60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="C61" t="s">
-        <v>62</v>
-      </c>
-      <c r="D61">
-        <v>0</v>
-      </c>
-      <c r="E61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="C62" t="s">
-        <v>63</v>
-      </c>
-      <c r="D62">
-        <v>0</v>
-      </c>
-      <c r="E62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="C63" t="s">
-        <v>64</v>
-      </c>
-      <c r="D63">
-        <v>0</v>
-      </c>
-      <c r="E63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" t="s">
-        <v>59</v>
-      </c>
-      <c r="B67" t="b">
-        <v>1</v>
-      </c>
-      <c r="C67" t="s">
-        <v>25</v>
-      </c>
-      <c r="D67">
-        <v>0</v>
-      </c>
-      <c r="E67">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E76"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
@@ -2118,7 +2110,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -2200,300 +2192,303 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" t="b">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" t="b">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" t="s">
         <v>37</v>
       </c>
-      <c r="B30" t="b">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B29" t="b">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
         <v>9</v>
       </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" t="s">
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
         <v>38</v>
       </c>
-      <c r="B32" t="b">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B31" t="b">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
         <v>9</v>
       </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" t="s">
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
         <v>39</v>
       </c>
-      <c r="B34" t="b">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="B33" t="b">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
         <v>9</v>
       </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" t="s">
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
         <v>40</v>
       </c>
-      <c r="B36" t="b">
-        <v>1</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="B35" t="b">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
         <v>9</v>
       </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" t="s">
         <v>48</v>
       </c>
-      <c r="B40" t="b">
-        <v>1</v>
+      <c r="B39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" t="b">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" t="b">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>77</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" t="b">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" t="b">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>54</v>
+      </c>
+      <c r="B50" t="b">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" t="s">
-        <v>50</v>
-      </c>
-      <c r="B43" t="b">
-        <v>1</v>
-      </c>
-      <c r="C43" t="s">
-        <v>16</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" t="s">
-        <v>51</v>
-      </c>
-      <c r="B45" t="b">
-        <v>1</v>
-      </c>
-      <c r="C45" t="s">
-        <v>79</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" t="s">
-        <v>52</v>
-      </c>
-      <c r="B47" t="b">
-        <v>1</v>
-      </c>
-      <c r="C47" t="s">
-        <v>16</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" t="s">
-        <v>53</v>
-      </c>
-      <c r="B49" t="b">
-        <v>1</v>
-      </c>
-      <c r="C49" t="s">
-        <v>16</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" t="s">
-        <v>54</v>
-      </c>
-      <c r="B51" t="b">
-        <v>1</v>
-      </c>
-      <c r="C51" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-      <c r="E51">
-        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" t="s">
         <v>42</v>
       </c>
-      <c r="B55" t="b">
-        <v>1</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="B54" t="b">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
         <v>12</v>
       </c>
-      <c r="D55">
-        <v>1</v>
-      </c>
-      <c r="E55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" t="s">
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
         <v>43</v>
       </c>
-      <c r="B57" t="b">
-        <v>1</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="B56" t="b">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
         <v>12</v>
       </c>
-      <c r="D57">
-        <v>1</v>
-      </c>
-      <c r="E57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" t="s">
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
         <v>44</v>
       </c>
-      <c r="B59" t="b">
-        <v>1</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="B58" t="b">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
         <v>12</v>
       </c>
-      <c r="D59">
-        <v>1</v>
-      </c>
-      <c r="E59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" t="s">
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
         <v>45</v>
       </c>
-      <c r="B61" t="b">
-        <v>1</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="B60" t="b">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s">
         <v>12</v>
       </c>
-      <c r="D61">
-        <v>1</v>
-      </c>
-      <c r="E61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" t="s">
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
         <v>46</v>
       </c>
-      <c r="B63" t="b">
-        <v>1</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="B62" t="b">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
         <v>12</v>
       </c>
-      <c r="D63">
-        <v>1</v>
-      </c>
-      <c r="E63">
-        <v>1</v>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="B66" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B67" t="b">
         <v>1</v>
@@ -2501,7 +2496,7 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B68" t="b">
         <v>1</v>
@@ -2509,34 +2504,37 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
+        <v>83</v>
+      </c>
+      <c r="B69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
         <v>84</v>
-      </c>
-      <c r="B69" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" t="s">
-        <v>85</v>
-      </c>
-      <c r="B70" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>86</v>
+        <v>18</v>
+      </c>
+      <c r="B72" t="b">
+        <v>1</v>
+      </c>
+      <c r="C72" t="s">
+        <v>20</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" t="s">
-        <v>18</v>
-      </c>
-      <c r="B73" t="b">
-        <v>1</v>
-      </c>
       <c r="C73" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -2547,7 +2545,7 @@
     </row>
     <row r="74" spans="1:5">
       <c r="C74" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -2558,23 +2556,12 @@
     </row>
     <row r="75" spans="1:5">
       <c r="C75" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D75">
         <v>1</v>
       </c>
       <c r="E75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="C76" t="s">
-        <v>23</v>
-      </c>
-      <c r="D76">
-        <v>1</v>
-      </c>
-      <c r="E76">
         <v>1</v>
       </c>
     </row>

</xml_diff>